<commit_message>
PMO-2093: implementation adjusted in order to apply similar principals as for CXL
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/QuotaShareEventLimit.xlsx
+++ b/test/data/spreadsheets/QuotaShareEventLimit.xlsx
@@ -83,10 +83,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +124,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +147,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -203,12 +217,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -227,9 +242,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -523,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V50"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -538,7 +559,7 @@
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -549,12 +570,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:24">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -574,7 +595,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -598,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -622,12 +643,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -653,7 +674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:24">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -701,7 +722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:24">
       <c r="A11" s="5">
         <v>0</v>
       </c>
@@ -717,23 +738,23 @@
       <c r="F11" s="16">
         <v>1000</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="19">
         <f>$F11*B$5</f>
         <v>800</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="20">
         <f t="shared" ref="H11:K11" si="2">$F11*C$5</f>
         <v>250</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="20">
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="20">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="20">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -757,8 +778,13 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="5">
         <v>0</v>
       </c>
@@ -778,23 +804,23 @@
       <c r="F12" s="16">
         <v>1500</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="19">
         <f t="shared" ref="G12:G18" si="5">$F12*B$5</f>
         <v>1200</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="20">
         <f t="shared" ref="H12:H18" si="6">$F12*C$5</f>
         <v>375</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="20">
         <f t="shared" ref="I12:I18" si="7">$F12*D$5</f>
         <v>-150</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="20">
         <f t="shared" ref="J12:J18" si="8">$F12*E$5</f>
         <v>37.5</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="20">
         <f t="shared" ref="K12:K18" si="9">$F12*F$5</f>
         <v>37.5</v>
       </c>
@@ -818,16 +844,15 @@
         <f t="shared" ref="P12:P18" si="14">$F12*F$6</f>
         <v>75</v>
       </c>
-      <c r="U12">
-        <f>550/750*0.3</f>
-        <v>0.21999999999999997</v>
-      </c>
-      <c r="V12">
-        <f>2500*U12</f>
-        <v>549.99999999999989</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -847,23 +872,23 @@
       <c r="F13" s="16">
         <v>2500</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="19">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="20">
         <f t="shared" si="6"/>
         <v>625</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="20">
         <f t="shared" si="7"/>
         <v>-250</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="20">
         <f t="shared" si="8"/>
         <v>62.5</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="20">
         <f t="shared" si="9"/>
         <v>62.5</v>
       </c>
@@ -887,8 +912,15 @@
         <f t="shared" si="14"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="5">
         <v>0</v>
       </c>
@@ -908,23 +940,23 @@
       <c r="F14" s="16">
         <v>2000</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="19">
         <f t="shared" si="5"/>
         <v>1600</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="20">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="20">
         <f t="shared" si="7"/>
         <v>-200</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="20">
         <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="20">
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
@@ -948,8 +980,14 @@
         <f t="shared" si="14"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="20"/>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -969,23 +1007,23 @@
       <c r="F15" s="16">
         <v>2500</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="19">
         <f t="shared" si="5"/>
         <v>2000</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="20">
         <f t="shared" si="6"/>
         <v>625</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="20">
         <f t="shared" si="7"/>
         <v>-250</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="20">
         <f t="shared" si="8"/>
         <v>62.5</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="20">
         <f t="shared" si="9"/>
         <v>62.5</v>
       </c>
@@ -1009,8 +1047,14 @@
         <f t="shared" si="14"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="20"/>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="5">
         <v>1</v>
       </c>
@@ -1026,23 +1070,23 @@
       <c r="F16" s="16">
         <v>4000</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="19">
         <f t="shared" si="5"/>
         <v>3200</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="20">
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="20">
         <f t="shared" si="7"/>
         <v>-400</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="20">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="20">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
@@ -1066,8 +1110,14 @@
         <f t="shared" si="14"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="20"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="5">
         <v>1</v>
       </c>
@@ -1087,23 +1137,23 @@
       <c r="F17" s="16">
         <v>3000</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="19">
         <f t="shared" si="5"/>
         <v>2400</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="20">
         <f t="shared" si="6"/>
         <v>750</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="20">
         <f t="shared" si="7"/>
         <v>-300</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="20">
         <f t="shared" si="8"/>
         <v>75</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="20">
         <f t="shared" si="9"/>
         <v>75</v>
       </c>
@@ -1127,8 +1177,14 @@
         <f t="shared" si="14"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="20"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -1148,23 +1204,23 @@
       <c r="F18" s="16">
         <v>3500</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="19">
         <f t="shared" si="5"/>
         <v>2800</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="20">
         <f t="shared" si="6"/>
         <v>875</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="20">
         <f t="shared" si="7"/>
         <v>-350</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="20">
         <f t="shared" si="8"/>
         <v>87.5</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="20">
         <f t="shared" si="9"/>
         <v>87.5</v>
       </c>
@@ -1188,13 +1244,22 @@
         <f t="shared" si="14"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="20"/>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="W19" s="21"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1202,7 +1267,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1210,7 +1275,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1218,7 +1283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +1315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:23">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1298,7 +1363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:23">
       <c r="A27" s="7">
         <v>0</v>
       </c>
@@ -1340,7 +1405,7 @@
         <v>30</v>
       </c>
       <c r="M27">
-        <f t="shared" ref="M27:M34" si="20">$F27*C$6</f>
+        <f t="shared" ref="M27:M32" si="20">$F27*C$6</f>
         <v>60</v>
       </c>
       <c r="N27">
@@ -1364,7 +1429,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:23">
       <c r="A28" s="7">
         <v>0</v>
       </c>
@@ -1382,29 +1447,27 @@
         <v>40969</v>
       </c>
       <c r="F28" s="11">
-        <f t="shared" ref="F28:F34" si="25">F12*$B$21</f>
+        <f t="shared" ref="F28:F32" si="25">F12*$B$21</f>
         <v>450</v>
       </c>
       <c r="G28" s="11">
         <f t="shared" ref="G28:G32" si="26">$F28*B$5</f>
         <v>360</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="17">
         <v>40</v>
       </c>
-      <c r="I28">
-        <v>-45</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="18"/>
-        <v>11.25</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="19"/>
-        <v>11.25</v>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+      <c r="J28" s="17">
+        <v>0</v>
+      </c>
+      <c r="K28" s="17">
+        <v>0</v>
       </c>
       <c r="L28" s="11">
-        <f t="shared" ref="L28:L34" si="27">$F28*B$6</f>
+        <f t="shared" ref="L28:L32" si="27">$F28*B$6</f>
         <v>45</v>
       </c>
       <c r="M28">
@@ -1419,19 +1482,19 @@
         <f t="shared" si="22"/>
         <v>135</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="17">
         <v>0</v>
       </c>
       <c r="R28" s="9">
         <f t="shared" ref="R28:R34" si="28">SUM(G28:K28)</f>
-        <v>377.5</v>
-      </c>
-      <c r="S28" s="9">
+        <v>400</v>
+      </c>
+      <c r="S28" s="18">
         <f t="shared" ref="S28:S34" si="29">SUM(L28:P28)</f>
         <v>427.5</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:23">
       <c r="A29" s="7">
         <v>0</v>
       </c>
@@ -1451,46 +1514,46 @@
       <c r="F29" s="11">
         <v>550</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="22">
         <v>600</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>-75</v>
-      </c>
-      <c r="J29">
-        <v>18.75</v>
-      </c>
-      <c r="K29">
-        <v>18.75</v>
-      </c>
-      <c r="L29" s="11">
+      <c r="H29" s="17">
+        <v>0</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="17">
+        <v>0</v>
+      </c>
+      <c r="K29" s="17">
+        <v>0</v>
+      </c>
+      <c r="L29" s="22">
         <v>75</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="17">
         <v>150</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="17">
         <v>262.5</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="17">
         <v>85</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="17">
         <v>0</v>
       </c>
       <c r="R29" s="9">
         <f t="shared" si="28"/>
-        <v>562.5</v>
-      </c>
-      <c r="S29" s="9">
+        <v>600</v>
+      </c>
+      <c r="S29" s="18">
         <f t="shared" si="29"/>
         <v>572.5</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:23">
       <c r="A30" s="7">
         <v>0</v>
       </c>
@@ -1560,7 +1623,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:23">
       <c r="A31" s="7">
         <v>1</v>
       </c>
@@ -1585,17 +1648,17 @@
         <f t="shared" si="26"/>
         <v>600</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>-75</v>
-      </c>
-      <c r="J31">
-        <v>18.75</v>
-      </c>
-      <c r="K31">
-        <v>18.75</v>
+      <c r="H31" s="17">
+        <v>0</v>
+      </c>
+      <c r="I31" s="17">
+        <v>0</v>
+      </c>
+      <c r="J31" s="17">
+        <v>0</v>
+      </c>
+      <c r="K31" s="17">
+        <v>0</v>
       </c>
       <c r="L31" s="11">
         <f t="shared" si="27"/>
@@ -1609,22 +1672,22 @@
         <f t="shared" si="21"/>
         <v>262.5</v>
       </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="R31" s="2">
+      <c r="O31" s="17">
+        <v>0</v>
+      </c>
+      <c r="P31" s="17">
+        <v>0</v>
+      </c>
+      <c r="R31" s="9">
         <f t="shared" si="28"/>
-        <v>562.5</v>
-      </c>
-      <c r="S31" s="2">
+        <v>600</v>
+      </c>
+      <c r="S31" s="18">
         <f t="shared" si="29"/>
         <v>487.5</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:23">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -1710,41 +1773,41 @@
       <c r="F33" s="11">
         <v>250</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="22">
         <v>400</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>-90</v>
-      </c>
-      <c r="J33">
-        <v>22.5</v>
-      </c>
-      <c r="K33">
-        <v>22.5</v>
-      </c>
-      <c r="L33" s="11">
+      <c r="H33" s="17">
+        <v>0</v>
+      </c>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+      <c r="J33" s="17">
+        <v>0</v>
+      </c>
+      <c r="K33" s="17">
+        <v>0</v>
+      </c>
+      <c r="L33" s="22">
         <v>90</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="17">
         <v>180</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="17">
         <v>242.5</v>
       </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="R33" s="2">
+      <c r="O33" s="17">
+        <v>0</v>
+      </c>
+      <c r="P33" s="17">
+        <v>0</v>
+      </c>
+      <c r="R33" s="9">
         <f t="shared" si="28"/>
-        <v>355</v>
-      </c>
-      <c r="S33" s="2">
+        <v>400</v>
+      </c>
+      <c r="S33" s="18">
         <f t="shared" si="29"/>
         <v>512.5</v>
       </c>
@@ -1773,24 +1836,24 @@
         <f>G18*$B$21</f>
         <v>840</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="17">
         <v>160</v>
       </c>
-      <c r="I34">
-        <v>-105</v>
-      </c>
-      <c r="J34">
-        <v>26.25</v>
-      </c>
-      <c r="K34">
-        <v>26.25</v>
+      <c r="I34" s="17">
+        <v>-2.5</v>
+      </c>
+      <c r="J34" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="K34" s="17">
+        <v>0</v>
       </c>
       <c r="L34" s="11">
         <f>L18*$B$21</f>
         <v>105</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:P34" si="30">M18*$B$21</f>
+        <f t="shared" ref="M34:O34" si="30">M18*$B$21</f>
         <v>210</v>
       </c>
       <c r="N34">
@@ -1801,12 +1864,12 @@
         <f t="shared" si="30"/>
         <v>315</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="17">
         <v>2.5</v>
       </c>
-      <c r="R34" s="2">
+      <c r="R34" s="9">
         <f t="shared" si="28"/>
-        <v>947.5</v>
+        <v>1000</v>
       </c>
       <c r="S34" s="2">
         <f t="shared" si="29"/>
@@ -2793,15 +2856,15 @@
       </c>
       <c r="I4">
         <f>Calc!I28</f>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f>Calc!J28</f>
-        <v>11.25</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <f>Calc!K28</f>
-        <v>11.25</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <f>Calc!L28</f>
@@ -2859,15 +2922,15 @@
       </c>
       <c r="I5">
         <f>Calc!I29</f>
-        <v>-75</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <f>Calc!J29</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f>Calc!K29</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <f>Calc!L29</f>
@@ -2991,15 +3054,15 @@
       </c>
       <c r="I7">
         <f>Calc!I31</f>
-        <v>-75</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f>Calc!J31</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <f>Calc!K31</f>
-        <v>18.75</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <f>Calc!L31</f>
@@ -3123,15 +3186,15 @@
       </c>
       <c r="I9">
         <f>Calc!I33</f>
-        <v>-90</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f>Calc!J33</f>
-        <v>22.5</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <f>Calc!K33</f>
-        <v>22.5</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f>Calc!L33</f>
@@ -3189,15 +3252,15 @@
       </c>
       <c r="I10">
         <f>Calc!I34</f>
-        <v>-105</v>
+        <v>-2.5</v>
       </c>
       <c r="J10">
         <f>Calc!J34</f>
-        <v>26.25</v>
+        <v>2.5</v>
       </c>
       <c r="K10">
         <f>Calc!K34</f>
-        <v>26.25</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <f>Calc!L34</f>

</xml_diff>